<commit_message>
Alterações no arquivo pbix e ppt
</commit_message>
<xml_diff>
--- a/Base_Produto.xlsx
+++ b/Base_Produto.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio Cavalcante\Desktop\Projeto_Power_BI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccavalcante\Documents\Power BI Desktop\aaa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09C615A-7CF2-4A36-8BE4-4779D1132578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4A549A48-1E91-4EAB-B0FE-E618600E7733}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$28</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
   <si>
     <t>LG</t>
   </si>
@@ -123,12 +122,6 @@
     <t>SMART TV 75' 4K</t>
   </si>
   <si>
-    <t>SMART WATCH MI</t>
-  </si>
-  <si>
-    <t>XIAOMI</t>
-  </si>
-  <si>
     <t>IPHONE XS</t>
   </si>
   <si>
@@ -247,12 +240,63 @@
   </si>
   <si>
     <t>PD1024</t>
+  </si>
+  <si>
+    <t>PD1025</t>
+  </si>
+  <si>
+    <t>PD1026</t>
+  </si>
+  <si>
+    <t>PD1027</t>
+  </si>
+  <si>
+    <t>REDMI NOTE 7</t>
+  </si>
+  <si>
+    <t>REDMI NOTE 8</t>
+  </si>
+  <si>
+    <t>REDMI NOTE 9</t>
+  </si>
+  <si>
+    <t>REDMI</t>
+  </si>
+  <si>
+    <t>SMART WATCH LG</t>
+  </si>
+  <si>
+    <t>PD1028</t>
+  </si>
+  <si>
+    <t>REDMI NOTE 10</t>
+  </si>
+  <si>
+    <t>PD1029</t>
+  </si>
+  <si>
+    <t>PD1030</t>
+  </si>
+  <si>
+    <t>GUITARRA STRINBERG</t>
+  </si>
+  <si>
+    <t>GUITARRA IBANEZ</t>
+  </si>
+  <si>
+    <t>STRINBERG</t>
+  </si>
+  <si>
+    <t>IBANEZ</t>
+  </si>
+  <si>
+    <t>GUITARRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,9 +326,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -600,10 +647,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE391F-8A57-4486-A1E1-CCF8D83A4EE8}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -620,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -629,15 +678,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -646,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1">
         <v>2600</v>
@@ -657,7 +706,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -666,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
         <v>2500</v>
@@ -677,7 +726,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -686,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>4500</v>
@@ -697,7 +746,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -706,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1">
         <v>1750</v>
@@ -717,7 +766,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -726,7 +775,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1">
         <v>1500</v>
@@ -737,7 +786,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -746,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
         <v>1400</v>
@@ -757,7 +806,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -766,7 +815,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1">
         <v>2300</v>
@@ -777,7 +826,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -786,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1">
         <v>2000</v>
@@ -797,7 +846,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -806,7 +855,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1">
         <v>1400</v>
@@ -817,7 +866,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
@@ -826,7 +875,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1">
         <v>1900</v>
@@ -837,7 +886,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
@@ -846,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1">
         <v>2000</v>
@@ -857,7 +906,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>21</v>
@@ -866,7 +915,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1">
         <v>5500</v>
@@ -877,7 +926,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
@@ -886,7 +935,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1">
         <v>1550</v>
@@ -897,7 +946,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
@@ -906,7 +955,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1">
         <v>1100</v>
@@ -917,7 +966,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -926,7 +975,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1">
         <v>700</v>
@@ -937,7 +986,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>27</v>
@@ -946,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1">
         <v>1450</v>
@@ -957,7 +1006,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -966,7 +1015,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1">
         <v>5200</v>
@@ -977,16 +1026,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1">
         <v>1200</v>
@@ -997,16 +1046,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1">
         <v>6500</v>
@@ -1017,16 +1066,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1">
         <v>1500</v>
@@ -1037,16 +1086,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1">
         <v>3000</v>
@@ -1057,16 +1106,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E23" s="1">
         <v>750</v>
@@ -1077,16 +1126,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1">
         <v>1500</v>
@@ -1097,16 +1146,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1">
         <v>2400</v>
@@ -1115,8 +1164,129 @@
         <v>1150</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1200</v>
+      </c>
+      <c r="F26" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1300</v>
+      </c>
+      <c r="F27" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F28" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1800</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2100</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F25" xr:uid="{73CC350E-DA58-4AD4-BB27-10AE1BFAC375}"/>
+  <autoFilter ref="A1:F28"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>